<commit_message>
Changed YPS to Bridge Mobile Phils. Inc.
</commit_message>
<xml_diff>
--- a/Business Plan Documents/YPS Twelve Month Profit and Loss Projection.xlsx
+++ b/Business Plan Documents/YPS Twelve Month Profit and Loss Projection.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Tentreps\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\tentrep-yps\Business Plan Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7935" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7935" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="PnL projection (Year 1)" sheetId="1" r:id="rId1"/>
@@ -594,9 +594,6 @@
     <t>% B/A</t>
   </si>
   <si>
-    <t>YPS</t>
-  </si>
-  <si>
     <t>Maintenance and Support</t>
   </si>
   <si>
@@ -712,6 +709,9 @@
   </si>
   <si>
     <t>Adj. to Retained Earnings</t>
+  </si>
+  <si>
+    <t>Bridge Mobile Phils, Inc.</t>
   </si>
 </sst>
 </file>
@@ -2185,7 +2185,7 @@
       <pane xSplit="1" ySplit="7" topLeftCell="K23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="AC28" sqref="AC28:AC35"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2241,7 +2241,7 @@
     </row>
     <row r="2" spans="1:28" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="D2" s="3"/>
       <c r="F2" s="3"/>
@@ -2438,7 +2438,7 @@
     </row>
     <row r="8" spans="1:28" s="18" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="20"/>
       <c r="C8" s="21">
@@ -2536,7 +2536,7 @@
     </row>
     <row r="9" spans="1:28" s="18" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="20"/>
       <c r="C9" s="21">
@@ -2634,7 +2634,7 @@
     </row>
     <row r="10" spans="1:28" s="18" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A10" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="23"/>
       <c r="C10" s="24">
@@ -2732,7 +2732,7 @@
     </row>
     <row r="11" spans="1:28" s="18" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A11" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="20"/>
       <c r="C11" s="21">
@@ -2830,7 +2830,7 @@
     </row>
     <row r="12" spans="1:28" s="18" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A12" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="20"/>
       <c r="C12" s="21">
@@ -3068,7 +3068,7 @@
     </row>
     <row r="15" spans="1:28" s="18" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="33"/>
       <c r="C15" s="15"/>
@@ -3100,7 +3100,7 @@
     </row>
     <row r="16" spans="1:28" s="18" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" s="36"/>
       <c r="C16" s="24">
@@ -3591,7 +3591,7 @@
     </row>
     <row r="25" spans="1:29" s="18" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A25" s="43" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B25" s="23"/>
       <c r="C25" s="15">
@@ -3689,7 +3689,7 @@
     </row>
     <row r="26" spans="1:29" s="18" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A26" s="43" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" s="23"/>
       <c r="C26" s="15"/>
@@ -3721,7 +3721,7 @@
     </row>
     <row r="27" spans="1:29" s="18" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="36" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B27" s="23"/>
       <c r="C27" s="24">
@@ -3914,7 +3914,7 @@
     </row>
     <row r="29" spans="1:29" s="18" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A29" s="36" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B29" s="23"/>
       <c r="C29" s="24">
@@ -4012,7 +4012,7 @@
     </row>
     <row r="30" spans="1:29" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="44" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30" s="23"/>
       <c r="C30" s="45">
@@ -4110,7 +4110,7 @@
     </row>
     <row r="31" spans="1:29" s="18" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A31" s="36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" s="23"/>
       <c r="C31" s="24">
@@ -4208,7 +4208,7 @@
     </row>
     <row r="32" spans="1:29" s="18" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A32" s="36" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B32" s="23"/>
       <c r="C32" s="24">
@@ -4306,7 +4306,7 @@
     </row>
     <row r="33" spans="1:28" s="18" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A33" s="36" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B33" s="23"/>
       <c r="C33" s="24">
@@ -4404,7 +4404,7 @@
     </row>
     <row r="34" spans="1:28" s="18" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A34" s="36" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B34" s="23"/>
       <c r="C34" s="24">
@@ -4496,7 +4496,7 @@
     </row>
     <row r="35" spans="1:28" s="18" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A35" s="36" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B35" s="23"/>
       <c r="C35" s="24">
@@ -4863,27 +4863,27 @@
     </row>
     <row r="54" spans="3:17" x14ac:dyDescent="0.2">
       <c r="E54" s="44" t="s">
+        <v>34</v>
+      </c>
+      <c r="F54" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="F54" s="50" t="s">
+      <c r="G54" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="G54" s="44" t="s">
-        <v>37</v>
-      </c>
       <c r="I54" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="M54" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="M54" s="44" t="s">
-        <v>41</v>
-      </c>
       <c r="Q54" s="50" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="55" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C55" s="44" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E55" s="44">
         <v>100000</v>
@@ -4903,7 +4903,7 @@
     </row>
     <row r="56" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C56" s="44" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D56" s="44"/>
       <c r="E56" s="44">
@@ -4926,7 +4926,7 @@
     </row>
     <row r="57" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C57" s="44" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D57" s="44"/>
       <c r="E57" s="44">
@@ -4959,32 +4959,32 @@
     </row>
     <row r="60" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C60" s="44" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D60" s="44"/>
       <c r="F60" s="44"/>
       <c r="N60" s="50" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="61" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C61" s="44" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D61" s="44"/>
       <c r="F61" s="44"/>
       <c r="N61" s="50" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="62" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C62" s="44" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D62" s="44"/>
       <c r="F62" s="44"/>
       <c r="N62" s="50" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="63" spans="3:17" x14ac:dyDescent="0.2">
@@ -5017,8 +5017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD71"/>
   <sheetViews>
-    <sheetView topLeftCell="I13" workbookViewId="0">
-      <selection activeCell="AA28" sqref="AA28:AA35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5062,7 +5062,7 @@
     </row>
     <row r="2" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="63" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="B2" s="61"/>
       <c r="C2" s="61"/>
@@ -5328,7 +5328,7 @@
     </row>
     <row r="8" spans="1:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="20"/>
       <c r="C8" s="55">
@@ -5428,7 +5428,7 @@
     </row>
     <row r="9" spans="1:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="20"/>
       <c r="C9" s="56">
@@ -5528,7 +5528,7 @@
     </row>
     <row r="10" spans="1:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="23"/>
       <c r="C10" s="56">
@@ -5628,7 +5628,7 @@
     </row>
     <row r="11" spans="1:30" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="20"/>
       <c r="C11" s="56">
@@ -5728,7 +5728,7 @@
     </row>
     <row r="12" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="20"/>
       <c r="C12" s="56">
@@ -5972,7 +5972,7 @@
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A15" s="57" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="33"/>
       <c r="C15" s="15"/>
@@ -6006,7 +6006,7 @@
     </row>
     <row r="16" spans="1:30" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" s="36"/>
       <c r="C16" s="24">
@@ -6514,7 +6514,7 @@
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A25" s="29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B25" s="23"/>
       <c r="C25" s="15">
@@ -6614,7 +6614,7 @@
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A26" s="29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" s="23"/>
       <c r="C26" s="15"/>
@@ -6648,7 +6648,7 @@
     </row>
     <row r="27" spans="1:30" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="36" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B27" s="23"/>
       <c r="C27" s="24">
@@ -6845,7 +6845,7 @@
     </row>
     <row r="29" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="36" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B29" s="23"/>
       <c r="C29" s="24">
@@ -6945,7 +6945,7 @@
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A30" s="58" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30" s="23"/>
       <c r="C30" s="59">
@@ -7045,7 +7045,7 @@
     </row>
     <row r="31" spans="1:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" s="23"/>
       <c r="C31" s="24">
@@ -7145,7 +7145,7 @@
     </row>
     <row r="32" spans="1:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="36" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B32" s="23"/>
       <c r="C32" s="24">
@@ -7245,7 +7245,7 @@
     </row>
     <row r="33" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="36" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B33" s="23"/>
       <c r="C33" s="24">
@@ -7345,7 +7345,7 @@
     </row>
     <row r="34" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="36" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B34" s="23"/>
       <c r="C34" s="24">
@@ -7439,7 +7439,7 @@
     </row>
     <row r="35" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="36" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B35" s="23"/>
       <c r="C35" s="24">
@@ -8279,29 +8279,29 @@
       <c r="C54" s="58"/>
       <c r="D54" s="66"/>
       <c r="E54" s="58" t="s">
+        <v>34</v>
+      </c>
+      <c r="F54" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="F54" s="66" t="s">
+      <c r="G54" s="58" t="s">
         <v>36</v>
-      </c>
-      <c r="G54" s="58" t="s">
-        <v>37</v>
       </c>
       <c r="H54" s="66"/>
       <c r="I54" s="58" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J54" s="66"/>
       <c r="K54" s="58"/>
       <c r="L54" s="66"/>
       <c r="M54" s="58" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N54" s="66"/>
       <c r="O54" s="58"/>
       <c r="P54" s="66"/>
       <c r="Q54" s="66" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="R54" s="66"/>
       <c r="S54" s="58"/>
@@ -8321,7 +8321,7 @@
       <c r="A55" s="61"/>
       <c r="B55" s="58"/>
       <c r="C55" s="58" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D55" s="66"/>
       <c r="E55" s="58">
@@ -8365,7 +8365,7 @@
       <c r="A56" s="61"/>
       <c r="B56" s="58"/>
       <c r="C56" s="58" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D56" s="58"/>
       <c r="E56" s="58">
@@ -8409,7 +8409,7 @@
       <c r="A57" s="61"/>
       <c r="B57" s="58"/>
       <c r="C57" s="58" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D57" s="58"/>
       <c r="E57" s="58">
@@ -8520,7 +8520,7 @@
       <c r="A60" s="61"/>
       <c r="B60" s="58"/>
       <c r="C60" s="58" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D60" s="58"/>
       <c r="E60" s="58"/>
@@ -8533,7 +8533,7 @@
       <c r="L60" s="66"/>
       <c r="M60" s="58"/>
       <c r="N60" s="66" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O60" s="58"/>
       <c r="P60" s="66"/>
@@ -8556,7 +8556,7 @@
       <c r="A61" s="61"/>
       <c r="B61" s="58"/>
       <c r="C61" s="58" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D61" s="58"/>
       <c r="E61" s="58"/>
@@ -8569,7 +8569,7 @@
       <c r="L61" s="66"/>
       <c r="M61" s="58"/>
       <c r="N61" s="66" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O61" s="58"/>
       <c r="P61" s="66"/>
@@ -8592,7 +8592,7 @@
       <c r="A62" s="61"/>
       <c r="B62" s="58"/>
       <c r="C62" s="58" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D62" s="58"/>
       <c r="E62" s="58"/>
@@ -8605,7 +8605,7 @@
       <c r="L62" s="66"/>
       <c r="M62" s="58"/>
       <c r="N62" s="66" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O62" s="58"/>
       <c r="P62" s="66"/>
@@ -8922,8 +8922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD71"/>
   <sheetViews>
-    <sheetView topLeftCell="K16" workbookViewId="0">
-      <selection activeCell="AA13" sqref="AA13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8968,7 +8968,7 @@
     </row>
     <row r="2" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -9234,7 +9234,7 @@
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="20"/>
       <c r="C8" s="70">
@@ -9334,7 +9334,7 @@
     </row>
     <row r="9" spans="1:30" ht="24" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="20"/>
       <c r="C9" s="93">
@@ -9434,7 +9434,7 @@
     </row>
     <row r="10" spans="1:30" ht="24" x14ac:dyDescent="0.2">
       <c r="A10" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="23"/>
       <c r="C10" s="94">
@@ -9534,7 +9534,7 @@
     </row>
     <row r="11" spans="1:30" ht="24" x14ac:dyDescent="0.2">
       <c r="A11" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="20"/>
       <c r="C11" s="117">
@@ -9634,7 +9634,7 @@
     </row>
     <row r="12" spans="1:30" ht="24" x14ac:dyDescent="0.2">
       <c r="A12" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="20"/>
       <c r="C12" s="130">
@@ -9878,7 +9878,7 @@
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A15" s="57" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="33"/>
       <c r="C15" s="15"/>
@@ -9912,7 +9912,7 @@
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" s="36"/>
       <c r="C16" s="24">
@@ -10420,7 +10420,7 @@
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A25" s="29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B25" s="23"/>
       <c r="C25" s="15">
@@ -10520,7 +10520,7 @@
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A26" s="29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" s="23"/>
       <c r="C26" s="15"/>
@@ -10554,7 +10554,7 @@
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A27" s="36" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B27" s="23"/>
       <c r="C27" s="24">
@@ -10751,7 +10751,7 @@
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A29" s="36" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B29" s="23"/>
       <c r="C29" s="24">
@@ -10851,7 +10851,7 @@
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A30" s="58" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30" s="23"/>
       <c r="C30" s="58">
@@ -10951,7 +10951,7 @@
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A31" s="36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" s="23"/>
       <c r="C31" s="24">
@@ -11051,7 +11051,7 @@
     </row>
     <row r="32" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A32" s="36" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B32" s="23"/>
       <c r="C32" s="24">
@@ -11151,7 +11151,7 @@
     </row>
     <row r="33" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A33" s="36" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B33" s="23"/>
       <c r="C33" s="24">
@@ -11251,7 +11251,7 @@
     </row>
     <row r="34" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A34" s="36" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B34" s="23"/>
       <c r="C34" s="24">
@@ -11345,7 +11345,7 @@
     </row>
     <row r="35" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A35" s="36" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B35" s="23"/>
       <c r="C35" s="24">
@@ -12185,29 +12185,29 @@
       <c r="C54" s="44"/>
       <c r="D54" s="50"/>
       <c r="E54" s="44" t="s">
+        <v>34</v>
+      </c>
+      <c r="F54" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="F54" s="50" t="s">
+      <c r="G54" s="44" t="s">
         <v>36</v>
-      </c>
-      <c r="G54" s="44" t="s">
-        <v>37</v>
       </c>
       <c r="H54" s="50"/>
       <c r="I54" s="44" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J54" s="50"/>
       <c r="K54" s="44"/>
       <c r="L54" s="50"/>
       <c r="M54" s="44" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N54" s="50"/>
       <c r="O54" s="44"/>
       <c r="P54" s="50"/>
       <c r="Q54" s="50" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="R54" s="50"/>
       <c r="S54" s="44"/>
@@ -12227,7 +12227,7 @@
       <c r="A55" s="51"/>
       <c r="B55" s="44"/>
       <c r="C55" s="44" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D55" s="50"/>
       <c r="E55" s="44">
@@ -12271,7 +12271,7 @@
       <c r="A56" s="51"/>
       <c r="B56" s="44"/>
       <c r="C56" s="44" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D56" s="44"/>
       <c r="E56" s="44">
@@ -12315,7 +12315,7 @@
       <c r="A57" s="51"/>
       <c r="B57" s="44"/>
       <c r="C57" s="44" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D57" s="44"/>
       <c r="E57" s="44">
@@ -12426,7 +12426,7 @@
       <c r="A60" s="51"/>
       <c r="B60" s="44"/>
       <c r="C60" s="44" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D60" s="44"/>
       <c r="E60" s="44"/>
@@ -12439,7 +12439,7 @@
       <c r="L60" s="50"/>
       <c r="M60" s="44"/>
       <c r="N60" s="50" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O60" s="44"/>
       <c r="P60" s="50"/>
@@ -12462,7 +12462,7 @@
       <c r="A61" s="51"/>
       <c r="B61" s="44"/>
       <c r="C61" s="44" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D61" s="44"/>
       <c r="E61" s="44"/>
@@ -12475,7 +12475,7 @@
       <c r="L61" s="50"/>
       <c r="M61" s="44"/>
       <c r="N61" s="50" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O61" s="44"/>
       <c r="P61" s="50"/>
@@ -12498,7 +12498,7 @@
       <c r="A62" s="51"/>
       <c r="B62" s="44"/>
       <c r="C62" s="44" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D62" s="44"/>
       <c r="E62" s="44"/>
@@ -12511,7 +12511,7 @@
       <c r="L62" s="50"/>
       <c r="M62" s="44"/>
       <c r="N62" s="50" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O62" s="44"/>
       <c r="P62" s="50"/>
@@ -12828,8 +12828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD67"/>
   <sheetViews>
-    <sheetView topLeftCell="K16" workbookViewId="0">
-      <selection activeCell="AA13" sqref="AA13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12875,7 +12875,7 @@
     </row>
     <row r="2" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -13141,7 +13141,7 @@
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="20"/>
       <c r="C8" s="132">
@@ -13241,7 +13241,7 @@
     </row>
     <row r="9" spans="1:30" ht="24" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="20"/>
       <c r="C9" s="155">
@@ -13341,7 +13341,7 @@
     </row>
     <row r="10" spans="1:30" ht="24" x14ac:dyDescent="0.2">
       <c r="A10" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="23"/>
       <c r="C10" s="156">
@@ -13441,7 +13441,7 @@
     </row>
     <row r="11" spans="1:30" ht="24" x14ac:dyDescent="0.2">
       <c r="A11" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="20"/>
       <c r="C11" s="179">
@@ -13541,7 +13541,7 @@
     </row>
     <row r="12" spans="1:30" ht="24" x14ac:dyDescent="0.2">
       <c r="A12" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="20"/>
       <c r="C12" s="180">
@@ -13785,7 +13785,7 @@
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A15" s="57" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="33"/>
       <c r="C15" s="15"/>
@@ -13819,7 +13819,7 @@
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" s="36"/>
       <c r="C16" s="24">
@@ -14327,7 +14327,7 @@
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A25" s="29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B25" s="23"/>
       <c r="C25" s="15">
@@ -14427,7 +14427,7 @@
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A26" s="29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" s="23"/>
       <c r="C26" s="15"/>
@@ -14461,7 +14461,7 @@
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A27" s="36" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B27" s="23"/>
       <c r="C27" s="24">
@@ -14658,7 +14658,7 @@
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A29" s="36" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B29" s="23"/>
       <c r="C29" s="24">
@@ -14758,7 +14758,7 @@
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A30" s="58" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30" s="23"/>
       <c r="C30" s="58">
@@ -14858,7 +14858,7 @@
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A31" s="36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" s="23"/>
       <c r="C31" s="24">
@@ -14958,7 +14958,7 @@
     </row>
     <row r="32" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A32" s="36" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B32" s="23"/>
       <c r="C32" s="24">
@@ -15058,7 +15058,7 @@
     </row>
     <row r="33" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A33" s="36" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B33" s="23"/>
       <c r="C33" s="24">
@@ -15158,7 +15158,7 @@
     </row>
     <row r="34" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A34" s="36" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B34" s="23"/>
       <c r="C34" s="24">
@@ -15252,7 +15252,7 @@
     </row>
     <row r="35" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A35" s="36" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B35" s="23"/>
       <c r="C35" s="24">
@@ -16092,29 +16092,29 @@
       <c r="C54" s="44"/>
       <c r="D54" s="50"/>
       <c r="E54" s="44" t="s">
+        <v>34</v>
+      </c>
+      <c r="F54" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="F54" s="50" t="s">
+      <c r="G54" s="44" t="s">
         <v>36</v>
-      </c>
-      <c r="G54" s="44" t="s">
-        <v>37</v>
       </c>
       <c r="H54" s="50"/>
       <c r="I54" s="44" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J54" s="50"/>
       <c r="K54" s="44"/>
       <c r="L54" s="50"/>
       <c r="M54" s="44" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N54" s="50"/>
       <c r="O54" s="44"/>
       <c r="P54" s="50"/>
       <c r="Q54" s="50" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="R54" s="50"/>
       <c r="S54" s="44"/>
@@ -16134,7 +16134,7 @@
       <c r="A55" s="51"/>
       <c r="B55" s="44"/>
       <c r="C55" s="44" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D55" s="50"/>
       <c r="E55" s="44">
@@ -16178,7 +16178,7 @@
       <c r="A56" s="51"/>
       <c r="B56" s="44"/>
       <c r="C56" s="44" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D56" s="44"/>
       <c r="E56" s="44">
@@ -16222,7 +16222,7 @@
       <c r="A57" s="51"/>
       <c r="B57" s="44"/>
       <c r="C57" s="44" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D57" s="44"/>
       <c r="E57" s="44">
@@ -16333,7 +16333,7 @@
       <c r="A60" s="51"/>
       <c r="B60" s="44"/>
       <c r="C60" s="44" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D60" s="44"/>
       <c r="E60" s="44"/>
@@ -16346,7 +16346,7 @@
       <c r="L60" s="50"/>
       <c r="M60" s="44"/>
       <c r="N60" s="50" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O60" s="44"/>
       <c r="P60" s="50"/>
@@ -16369,7 +16369,7 @@
       <c r="A61" s="51"/>
       <c r="B61" s="44"/>
       <c r="C61" s="44" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D61" s="44"/>
       <c r="E61" s="44"/>
@@ -16382,7 +16382,7 @@
       <c r="L61" s="50"/>
       <c r="M61" s="44"/>
       <c r="N61" s="50" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O61" s="44"/>
       <c r="P61" s="50"/>
@@ -16405,7 +16405,7 @@
       <c r="A62" s="51"/>
       <c r="B62" s="44"/>
       <c r="C62" s="44" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D62" s="44"/>
       <c r="E62" s="44"/>
@@ -16418,7 +16418,7 @@
       <c r="L62" s="50"/>
       <c r="M62" s="44"/>
       <c r="N62" s="50" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O62" s="44"/>
       <c r="P62" s="50"/>
@@ -16607,7 +16607,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -16643,7 +16643,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="131" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B3" s="196">
         <v>13604200</v>
@@ -16678,7 +16678,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="197" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4" s="198">
         <v>1108</v>
@@ -16770,7 +16770,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="207" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="209">
         <v>1870000</v>
@@ -16809,7 +16809,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="207" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="196">
         <v>0</v>
@@ -16848,7 +16848,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="207" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" s="196">
         <v>0</v>
@@ -16926,7 +16926,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="207" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="196">
         <v>57600</v>
@@ -16965,7 +16965,7 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="208" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" s="196">
         <v>72088</v>
@@ -17004,7 +17004,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="207" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" s="196">
         <v>12000</v>
@@ -17043,7 +17043,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="207" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15" s="196">
         <v>15588</v>
@@ -17082,7 +17082,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="207" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" s="196">
         <v>42000</v>
@@ -17121,7 +17121,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="207" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17" s="196">
         <v>24000</v>
@@ -17160,7 +17160,7 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="207" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" s="196">
         <v>20000</v>
@@ -17243,7 +17243,7 @@
     <row r="20" spans="1:16" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="131" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B21" s="196">
         <f>B5-B19</f>
@@ -17272,7 +17272,7 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="131" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B22" s="196">
         <v>3611024.96</v>
@@ -17297,7 +17297,7 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="131" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B23" s="196">
         <f>B21-B22</f>
@@ -17326,7 +17326,7 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="131" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B24" s="196">
         <v>0</v>
@@ -17351,7 +17351,7 @@
     </row>
     <row r="25" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="131" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B25" s="216">
         <f>B23-B24</f>

</xml_diff>